<commit_message>
Run Problemas: 016 requests+SSL, 018 fallback historicos, Paraguay uc-chrome, workflow y run_problemas solo 5 scripts
Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/update/historicos/dolar_bevsa_uyu_temp.xlsx
+++ b/update/historicos/dolar_bevsa_uyu_temp.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -499,548 +499,574 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>46059</v>
+        <v>46063</v>
       </c>
       <c r="B3" t="n">
-        <v>38.516</v>
+        <v>38.469</v>
       </c>
       <c r="C3" t="n">
-        <v>38.516</v>
+        <v>38.469</v>
       </c>
       <c r="D3" t="n">
-        <v>38.56</v>
+        <v>38.48</v>
       </c>
       <c r="E3" t="n">
-        <v>38.55</v>
+        <v>38.45</v>
       </c>
       <c r="F3" t="n">
-        <v>38.6</v>
+        <v>38.49</v>
       </c>
       <c r="G3" t="n">
-        <v>70</v>
+        <v>28</v>
       </c>
       <c r="H3" t="n">
-        <v>35000000</v>
+        <v>14500000</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>46058</v>
+        <v>46062</v>
       </c>
       <c r="B4" t="n">
-        <v>38.776</v>
+        <v>38.364</v>
       </c>
       <c r="C4" t="n">
-        <v>38.776</v>
+        <v>38.364</v>
       </c>
       <c r="D4" t="n">
-        <v>38.68</v>
+        <v>38.4</v>
       </c>
       <c r="E4" t="n">
-        <v>38.65</v>
+        <v>38.38</v>
       </c>
       <c r="F4" t="n">
-        <v>38.72</v>
+        <v>38.44</v>
       </c>
       <c r="G4" t="n">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="H4" t="n">
-        <v>33300000</v>
+        <v>44000000</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>46057</v>
+        <v>46059</v>
       </c>
       <c r="B5" t="n">
-        <v>38.641</v>
+        <v>38.516</v>
       </c>
       <c r="C5" t="n">
-        <v>38.641</v>
+        <v>38.516</v>
       </c>
       <c r="D5" t="n">
-        <v>38.75</v>
+        <v>38.56</v>
       </c>
       <c r="E5" t="n">
-        <v>38.7</v>
+        <v>38.55</v>
       </c>
       <c r="F5" t="n">
-        <v>38.8</v>
+        <v>38.6</v>
       </c>
       <c r="G5" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="H5" t="n">
-        <v>30000000</v>
+        <v>35000000</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>46056</v>
+        <v>46058</v>
       </c>
       <c r="B6" t="n">
-        <v>38.566</v>
+        <v>38.776</v>
       </c>
       <c r="C6" t="n">
-        <v>38.566</v>
+        <v>38.776</v>
       </c>
       <c r="D6" t="n">
-        <v>38.58</v>
+        <v>38.68</v>
       </c>
       <c r="E6" t="n">
-        <v>38.57</v>
+        <v>38.65</v>
       </c>
       <c r="F6" t="n">
-        <v>38.59</v>
+        <v>38.72</v>
       </c>
       <c r="G6" t="n">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="H6" t="n">
-        <v>23500000</v>
+        <v>33300000</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>46055</v>
+        <v>46057</v>
       </c>
       <c r="B7" t="n">
-        <v>38.523</v>
+        <v>38.641</v>
       </c>
       <c r="C7" t="n">
-        <v>38.523</v>
+        <v>38.641</v>
       </c>
       <c r="D7" t="n">
-        <v>38.57</v>
+        <v>38.75</v>
       </c>
       <c r="E7" t="n">
-        <v>38.55</v>
+        <v>38.7</v>
       </c>
       <c r="F7" t="n">
-        <v>38.6</v>
+        <v>38.8</v>
       </c>
       <c r="G7" t="n">
-        <v>92</v>
+        <v>60</v>
       </c>
       <c r="H7" t="n">
-        <v>46500000</v>
+        <v>30000000</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>46052</v>
+        <v>46056</v>
       </c>
       <c r="B8" t="n">
-        <v>38.5</v>
+        <v>38.566</v>
       </c>
       <c r="C8" t="n">
-        <v>38.5</v>
+        <v>38.566</v>
       </c>
       <c r="D8" t="n">
-        <v>38.52</v>
+        <v>38.58</v>
       </c>
       <c r="E8" t="n">
-        <v>38.48</v>
+        <v>38.57</v>
       </c>
       <c r="F8" t="n">
-        <v>38.53</v>
+        <v>38.59</v>
       </c>
       <c r="G8" t="n">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="H8" t="n">
-        <v>38800000</v>
+        <v>23500000</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>46051</v>
+        <v>46055</v>
       </c>
       <c r="B9" t="n">
-        <v>38.784</v>
+        <v>38.523</v>
       </c>
       <c r="C9" t="n">
-        <v>38.784</v>
+        <v>38.523</v>
       </c>
       <c r="D9" t="n">
-        <v>38.65</v>
+        <v>38.57</v>
       </c>
       <c r="E9" t="n">
+        <v>38.55</v>
+      </c>
+      <c r="F9" t="n">
         <v>38.6</v>
       </c>
-      <c r="F9" t="n">
-        <v>38.75</v>
-      </c>
       <c r="G9" t="n">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="H9" t="n">
-        <v>59800000</v>
+        <v>46500000</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>46050</v>
+        <v>46052</v>
       </c>
       <c r="B10" t="n">
-        <v>38.793</v>
+        <v>38.5</v>
       </c>
       <c r="C10" t="n">
-        <v>38.793</v>
+        <v>38.5</v>
       </c>
       <c r="D10" t="n">
-        <v>38.9</v>
+        <v>38.52</v>
       </c>
       <c r="E10" t="n">
-        <v>38.87</v>
+        <v>38.48</v>
       </c>
       <c r="F10" t="n">
-        <v>38.95</v>
+        <v>38.53</v>
       </c>
       <c r="G10" t="n">
-        <v>51</v>
+        <v>78</v>
       </c>
       <c r="H10" t="n">
-        <v>25400000</v>
+        <v>38800000</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>46049</v>
+        <v>46051</v>
       </c>
       <c r="B11" t="n">
-        <v>37.983</v>
+        <v>38.784</v>
       </c>
       <c r="C11" t="n">
-        <v>37.983</v>
+        <v>38.784</v>
       </c>
       <c r="D11" t="n">
-        <v>38.3</v>
+        <v>38.65</v>
       </c>
       <c r="E11" t="n">
-        <v>38.2</v>
+        <v>38.6</v>
       </c>
       <c r="F11" t="n">
-        <v>38.45</v>
+        <v>38.75</v>
       </c>
       <c r="G11" t="n">
-        <v>83</v>
+        <v>116</v>
       </c>
       <c r="H11" t="n">
-        <v>40200000</v>
+        <v>59800000</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>46048</v>
+        <v>46050</v>
       </c>
       <c r="B12" t="n">
-        <v>37.831</v>
+        <v>38.793</v>
       </c>
       <c r="C12" t="n">
-        <v>37.831</v>
+        <v>38.793</v>
       </c>
       <c r="D12" t="n">
-        <v>37.8</v>
+        <v>38.9</v>
       </c>
       <c r="E12" t="n">
-        <v>37.73</v>
+        <v>38.87</v>
       </c>
       <c r="F12" t="n">
-        <v>37.82</v>
+        <v>38.95</v>
       </c>
       <c r="G12" t="n">
-        <v>121</v>
+        <v>51</v>
       </c>
       <c r="H12" t="n">
-        <v>63000000</v>
+        <v>25400000</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>46045</v>
+        <v>46049</v>
       </c>
       <c r="B13" t="n">
-        <v>37.454</v>
+        <v>37.983</v>
       </c>
       <c r="C13" t="n">
-        <v>37.454</v>
+        <v>37.983</v>
       </c>
       <c r="D13" t="n">
-        <v>38</v>
+        <v>38.3</v>
       </c>
       <c r="E13" t="n">
-        <v>38</v>
+        <v>38.2</v>
       </c>
       <c r="F13" t="n">
-        <v>38.15</v>
+        <v>38.45</v>
       </c>
       <c r="G13" t="n">
-        <v>163</v>
+        <v>83</v>
       </c>
       <c r="H13" t="n">
-        <v>83100000</v>
+        <v>40200000</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>46044</v>
+        <v>46048</v>
       </c>
       <c r="B14" t="n">
-        <v>37.512</v>
+        <v>37.831</v>
       </c>
       <c r="C14" t="n">
-        <v>37.512</v>
+        <v>37.831</v>
       </c>
       <c r="D14" t="n">
-        <v>37.3</v>
+        <v>37.8</v>
       </c>
       <c r="E14" t="n">
-        <v>37.25</v>
+        <v>37.73</v>
       </c>
       <c r="F14" t="n">
-        <v>37.35</v>
+        <v>37.82</v>
       </c>
       <c r="G14" t="n">
-        <v>50</v>
+        <v>121</v>
       </c>
       <c r="H14" t="n">
-        <v>26400000</v>
+        <v>63000000</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>46043</v>
+        <v>46045</v>
       </c>
       <c r="B15" t="n">
-        <v>37.854</v>
+        <v>37.454</v>
       </c>
       <c r="C15" t="n">
-        <v>37.854</v>
+        <v>37.454</v>
       </c>
       <c r="D15" t="n">
-        <v>37.8</v>
+        <v>38</v>
       </c>
       <c r="E15" t="n">
-        <v>37.75</v>
+        <v>38</v>
       </c>
       <c r="F15" t="n">
-        <v>37.85</v>
+        <v>38.15</v>
       </c>
       <c r="G15" t="n">
-        <v>71</v>
+        <v>163</v>
       </c>
       <c r="H15" t="n">
-        <v>35700000</v>
+        <v>83100000</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>46042</v>
+        <v>46044</v>
       </c>
       <c r="B16" t="n">
-        <v>38.218</v>
+        <v>37.512</v>
       </c>
       <c r="C16" t="n">
-        <v>38.218</v>
+        <v>37.512</v>
       </c>
       <c r="D16" t="n">
-        <v>38.18</v>
+        <v>37.3</v>
       </c>
       <c r="E16" t="n">
-        <v>38.18</v>
+        <v>37.25</v>
       </c>
       <c r="F16" t="n">
-        <v>38.22</v>
+        <v>37.35</v>
       </c>
       <c r="G16" t="n">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="H16" t="n">
-        <v>37500000</v>
+        <v>26400000</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>46041</v>
+        <v>46043</v>
       </c>
       <c r="B17" t="n">
-        <v>38.349</v>
+        <v>37.854</v>
       </c>
       <c r="C17" t="n">
-        <v>38.349</v>
+        <v>37.854</v>
       </c>
       <c r="D17" t="n">
-        <v>38.31</v>
+        <v>37.8</v>
       </c>
       <c r="E17" t="n">
-        <v>38.31</v>
+        <v>37.75</v>
       </c>
       <c r="F17" t="n">
-        <v>38.34</v>
+        <v>37.85</v>
       </c>
       <c r="G17" t="n">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="H17" t="n">
-        <v>11000000</v>
+        <v>35700000</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>46038</v>
+        <v>46042</v>
       </c>
       <c r="B18" t="n">
-        <v>38.415</v>
+        <v>38.218</v>
       </c>
       <c r="C18" t="n">
-        <v>38.415</v>
+        <v>38.218</v>
       </c>
       <c r="D18" t="n">
-        <v>38.45</v>
+        <v>38.18</v>
       </c>
       <c r="E18" t="n">
-        <v>38.4</v>
+        <v>38.18</v>
       </c>
       <c r="F18" t="n">
-        <v>38.45</v>
+        <v>38.22</v>
       </c>
       <c r="G18" t="n">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="H18" t="n">
-        <v>22000000</v>
+        <v>37500000</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>46037</v>
+        <v>46041</v>
       </c>
       <c r="B19" t="n">
-        <v>38.599</v>
+        <v>38.349</v>
       </c>
       <c r="C19" t="n">
-        <v>38.599</v>
+        <v>38.349</v>
       </c>
       <c r="D19" t="n">
-        <v>38.55</v>
+        <v>38.31</v>
       </c>
       <c r="E19" t="n">
-        <v>38.51</v>
+        <v>38.31</v>
       </c>
       <c r="F19" t="n">
-        <v>38.55</v>
+        <v>38.34</v>
       </c>
       <c r="G19" t="n">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="H19" t="n">
-        <v>18500000</v>
+        <v>11000000</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>46036</v>
+        <v>46038</v>
       </c>
       <c r="B20" t="n">
-        <v>38.685</v>
+        <v>38.415</v>
       </c>
       <c r="C20" t="n">
-        <v>38.685</v>
+        <v>38.415</v>
       </c>
       <c r="D20" t="n">
-        <v>38.65</v>
+        <v>38.45</v>
       </c>
       <c r="E20" t="n">
-        <v>38.62</v>
+        <v>38.4</v>
       </c>
       <c r="F20" t="n">
-        <v>38.65</v>
+        <v>38.45</v>
       </c>
       <c r="G20" t="n">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="H20" t="n">
-        <v>28900000</v>
+        <v>22000000</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>46035</v>
+        <v>46037</v>
       </c>
       <c r="B21" t="n">
-        <v>38.597</v>
+        <v>38.599</v>
       </c>
       <c r="C21" t="n">
-        <v>38.597</v>
+        <v>38.599</v>
       </c>
       <c r="D21" t="n">
-        <v>38.7</v>
+        <v>38.55</v>
       </c>
       <c r="E21" t="n">
-        <v>38.7</v>
+        <v>38.51</v>
       </c>
       <c r="F21" t="n">
-        <v>38.75</v>
+        <v>38.55</v>
       </c>
       <c r="G21" t="n">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="H21" t="n">
-        <v>33500000</v>
+        <v>18500000</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>46034</v>
+        <v>46036</v>
       </c>
       <c r="B22" t="n">
-        <v>38.72</v>
+        <v>38.685</v>
       </c>
       <c r="C22" t="n">
-        <v>38.72</v>
+        <v>38.685</v>
       </c>
       <c r="D22" t="n">
-        <v>38.68</v>
+        <v>38.65</v>
       </c>
       <c r="E22" t="n">
+        <v>38.62</v>
+      </c>
+      <c r="F22" t="n">
         <v>38.65</v>
       </c>
-      <c r="F22" t="n">
-        <v>38.73</v>
-      </c>
       <c r="G22" t="n">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="H22" t="n">
-        <v>33000000</v>
+        <v>28900000</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>46031</v>
+        <v>46035</v>
       </c>
       <c r="B23" t="n">
-        <v>38.815</v>
+        <v>38.597</v>
       </c>
       <c r="C23" t="n">
-        <v>38.815</v>
+        <v>38.597</v>
       </c>
       <c r="D23" t="n">
-        <v>38.79</v>
+        <v>38.7</v>
       </c>
       <c r="E23" t="n">
-        <v>38.79</v>
+        <v>38.7</v>
       </c>
       <c r="F23" t="n">
-        <v>38.82</v>
+        <v>38.75</v>
       </c>
       <c r="G23" t="n">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="H23" t="n">
-        <v>19000000</v>
+        <v>33500000</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="n">
+        <v>46034</v>
+      </c>
+      <c r="B24" t="n">
+        <v>38.72</v>
+      </c>
+      <c r="C24" t="n">
+        <v>38.72</v>
+      </c>
+      <c r="D24" t="n">
+        <v>38.68</v>
+      </c>
+      <c r="E24" t="n">
+        <v>38.65</v>
+      </c>
+      <c r="F24" t="n">
+        <v>38.73</v>
+      </c>
+      <c r="G24" t="n">
+        <v>58</v>
+      </c>
+      <c r="H24" t="n">
+        <v>33000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>